<commit_message>
Corrected number format support and handling of: - a few specific date formats, this is non-generic handling as of yet. - Percentage handling initial setup, works so far for some use cases.
</commit_message>
<xml_diff>
--- a/ExcelToWiki/exceltowiki/example/test.xlsx
+++ b/ExcelToWiki/exceltowiki/example/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32700" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="-460" yWindow="4120" windowWidth="33600" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,6 +86,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="172" formatCode="0.0000%"/>
+    <numFmt numFmtId="173" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -202,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -224,6 +229,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -559,7 +567,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -607,6 +615,15 @@
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="B3" s="15">
+        <v>42309</v>
+      </c>
+      <c r="C3" s="13">
+        <v>42309.604166666664</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.91323449999999995</v>
       </c>
     </row>
     <row r="4" spans="1:5">

</xml_diff>

<commit_message>
Inline double-pipe separator had a bug where a newline in the cell requires the wiki table to use a single pipe character. Updated the test.xlsx containing above situaion.
</commit_message>
<xml_diff>
--- a/ExcelToWiki/exceltowiki/example/test.xlsx
+++ b/ExcelToWiki/exceltowiki/example/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-460" yWindow="4120" windowWidth="33600" windowHeight="20480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Test Bold</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Test italics</t>
+  </si>
+  <si>
+    <t>test123</t>
   </si>
 </sst>
 </file>
@@ -87,11 +90,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
-    <numFmt numFmtId="172" formatCode="0.0000%"/>
-    <numFmt numFmtId="173" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,8 +158,16 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +204,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -203,11 +220,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -216,10 +234,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -229,11 +247,13 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -566,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -605,7 +625,7 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E2" t="s">
@@ -616,13 +636,13 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="11">
         <v>42309</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="9">
         <v>42309.604166666664</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="10">
         <v>0.91323449999999995</v>
       </c>
     </row>
@@ -630,34 +650,34 @@
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="13"/>
       <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="11"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="13"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
@@ -668,9 +688,15 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="15" t="s">
         <v>18</v>
       </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added better date format sensing.
</commit_message>
<xml_diff>
--- a/ExcelToWiki/exceltowiki/example/test.xlsx
+++ b/ExcelToWiki/exceltowiki/example/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-29500" yWindow="2480" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,10 +89,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="169" formatCode="ddd\ mm/d/yy"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -225,7 +226,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -237,7 +238,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -247,10 +260,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -587,7 +597,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -605,7 +615,7 @@
       <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -636,7 +646,7 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="14">
         <v>42309</v>
       </c>
       <c r="C3" s="9">
@@ -644,40 +654,43 @@
       </c>
       <c r="D3" s="10">
         <v>0.91323449999999995</v>
+      </c>
+      <c r="E3" s="19">
+        <v>42502</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="17"/>
       <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="13"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="17"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
@@ -688,15 +701,15 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>